<commit_message>
starting work on new density function
</commit_message>
<xml_diff>
--- a/resources/Test_Simulationen_4.xlsx
+++ b/resources/Test_Simulationen_4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\Programme\Physics-Capacitor-Simualtion\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10DDC372-6998-4D1C-B26F-411A90832482}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E2A5FDE-7A34-40B8-86EA-FE0156769421}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>name</t>
   </si>
@@ -79,9 +79,6 @@
   </si>
   <si>
     <t>0.032</t>
-  </si>
-  <si>
-    <t>Test_0_032_d_16_nbins_30</t>
   </si>
   <si>
     <t>Test_0_032_d_16_nbins_30_static</t>
@@ -414,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,15 +466,15 @@
         <v>11</v>
       </c>
       <c r="M1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" t="s">
         <v>20</v>
-      </c>
-      <c r="N1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2">
         <v>16</v>
@@ -517,50 +514,6 @@
       </c>
       <c r="N2" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3">
-        <v>16</v>
-      </c>
-      <c r="C3">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3" t="s">
-        <v>16</v>
-      </c>
-      <c r="L3">
-        <v>50</v>
-      </c>
-      <c r="M3">
-        <v>30</v>
-      </c>
-      <c r="N3" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>